<commit_message>
-Changed years for CRP
</commit_message>
<xml_diff>
--- a/data/AGE-WELL RFP Project Budget.xlsx
+++ b/data/AGE-WELL RFP Project Budget.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Budget" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Total</t>
   </si>
@@ -83,14 +83,6 @@
   <si>
     <t>Year 3
 (Apr 1, 2022 - Mar 31, 2023)</t>
-  </si>
-  <si>
-    <t>Year 4
-(Apr 1, 2023 - Mar 31, 2024)</t>
-  </si>
-  <si>
-    <t>Year 5
-(Apr 1, 2024 - Mar 31, 2025)</t>
   </si>
   <si>
     <t xml:space="preserve">** To estimate in-kind contributions, use CIHR In Kind Eligibility guidelines (http://www.cihr-irsc.gc.ca/e/3758.html). </t>
@@ -107,7 +99,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -307,7 +299,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -325,17 +317,17 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -668,33 +660,36 @@
   <dimension ref="A1:Z26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.42578125" style="1" customWidth="1"/>
-    <col min="2" max="14" width="13.28515625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12" style="1" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="12.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="9.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="7.140625" style="1" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="10" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="10" width="13.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12" style="1" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="7.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="10" style="1" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" style="1" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="7.140625" style="1" hidden="1" customWidth="1"/>
+    <col min="21" max="22" width="10" style="1" hidden="1" customWidth="1"/>
     <col min="23" max="23" width="12.42578125" style="1" hidden="1"/>
     <col min="24" max="24" width="7.140625" style="1" hidden="1"/>
     <col min="25" max="26" width="10" style="1" hidden="1"/>
     <col min="27" max="16384" width="9.140625" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>14</v>
       </c>
@@ -705,7 +700,7 @@
       <c r="I2" s="23"/>
       <c r="J2" s="23"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>15</v>
       </c>
@@ -716,7 +711,7 @@
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
     </row>
-    <row r="4" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="25" t="s">
         <v>16</v>
@@ -739,16 +734,8 @@
         <v>21</v>
       </c>
       <c r="J4" s="28"/>
-      <c r="K4" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="28"/>
-      <c r="M4" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="N4" s="28"/>
-    </row>
-    <row r="5" spans="1:22" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:18" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="26"/>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
@@ -770,20 +757,8 @@
       <c r="J5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M5" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N5" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -796,21 +771,17 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="19">
-        <f>SUM(E7,G7,I7,K7,M7)</f>
+        <f>SUM(E7,G7,I7)</f>
         <v>0</v>
       </c>
       <c r="C7" s="14">
-        <f>SUM(F7,H7,J7,L7,N7)</f>
+        <f>SUM(F7,H7,J7)</f>
         <v>0</v>
       </c>
       <c r="D7" s="14">
@@ -823,21 +794,17 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="19">
-        <f>SUM(E8,G8,I8,K8,M8)</f>
+        <f>SUM(E8,G8,I8)</f>
         <v>0</v>
       </c>
       <c r="C8" s="14">
-        <f>SUM(F8,H8,J8,L8,N8)</f>
+        <f t="shared" ref="C8:C9" si="0">SUM(F8,H8,J8)</f>
         <v>0</v>
       </c>
       <c r="D8" s="14">
@@ -850,21 +817,17 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="19">
-        <f>SUM(E9,G9,I9,K9,M9)</f>
+        <f>SUM(E9,G9,I9)</f>
         <v>0</v>
       </c>
       <c r="C9" s="14">
-        <f>SUM(F9,H9,J9,L9,N9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D9" s="14">
@@ -877,12 +840,8 @@
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-    </row>
-    <row r="10" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -895,21 +854,17 @@
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
       <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-    </row>
-    <row r="11" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="19">
-        <f>SUM(E11,G11,I11,K11,M11)</f>
+        <f>SUM(E11,G11,I11)</f>
         <v>0</v>
       </c>
       <c r="C11" s="14">
-        <f>SUM(F11,H11,J11,L11,N11)</f>
+        <f>SUM(F11,H11,J11)</f>
         <v>0</v>
       </c>
       <c r="D11" s="14">
@@ -922,25 +877,21 @@
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-    </row>
-    <row r="12" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="19">
-        <f>SUM(E12,G12,I12,K12,M12)</f>
+        <f t="shared" ref="B12:B16" si="1">SUM(E12,G12,I12)</f>
         <v>0</v>
       </c>
       <c r="C12" s="14">
-        <f>SUM(F12,H12,J12,L12,N12)</f>
+        <f t="shared" ref="C12:C16" si="2">SUM(F12,H12,J12)</f>
         <v>0</v>
       </c>
       <c r="D12" s="14">
-        <f t="shared" ref="D12:D15" si="0">B12+C12</f>
+        <f t="shared" ref="D12:D15" si="3">B12+C12</f>
         <v>0</v>
       </c>
       <c r="E12" s="14"/>
@@ -949,21 +900,17 @@
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-    </row>
-    <row r="13" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="19">
-        <f>SUM(E13,G13,I13,K13,M13)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C13" s="14">
-        <f>SUM(F13,H13,J13,L13,N13)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D13" s="14">
@@ -976,33 +923,29 @@
       <c r="H13" s="15"/>
       <c r="I13" s="15"/>
       <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
       <c r="O13" s="11"/>
       <c r="P13" s="11"/>
       <c r="Q13" s="11"/>
       <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="11"/>
-    </row>
-    <row r="14" spans="1:22" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:18" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="19">
-        <f>SUM(E14,G14,I14,K14,M14)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C14" s="14">
-        <f>SUM(F14,H14,J14,L14,N14)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D14" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E14" s="15"/>
@@ -1011,33 +954,29 @@
       <c r="H14" s="15"/>
       <c r="I14" s="15"/>
       <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
       <c r="O14" s="11"/>
       <c r="P14" s="11"/>
       <c r="Q14" s="11"/>
       <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="11"/>
-    </row>
-    <row r="15" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" s="19">
-        <f>SUM(E15,G15,I15,K15,M15)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C15" s="14">
-        <f>SUM(F15,H15,J15,L15,N15)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D15" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E15" s="15"/>
@@ -1046,21 +985,17 @@
       <c r="H15" s="15"/>
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-    </row>
-    <row r="16" spans="1:22" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B16" s="19">
-        <f>SUM(E16,G16,I16,K16,M16)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C16" s="14">
-        <f>SUM(F16,H16,J16,L16,N16)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D16" s="14">
@@ -1073,12 +1008,8 @@
       <c r="H16" s="15"/>
       <c r="I16" s="15"/>
       <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-    </row>
-    <row r="17" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>0</v>
       </c>
@@ -1099,43 +1030,27 @@
         <v>0</v>
       </c>
       <c r="F17" s="16">
-        <f t="shared" ref="F17:I17" si="1">SUM(F7:F9,F11:F16)</f>
+        <f t="shared" ref="F17:I17" si="4">SUM(F7:F9,F11:F16)</f>
         <v>0</v>
       </c>
       <c r="G17" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H17" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I17" s="16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J17" s="16">
-        <f t="shared" ref="J17" si="2">SUM(J7:J9,J11:J16)</f>
-        <v>0</v>
-      </c>
-      <c r="K17" s="16">
-        <f t="shared" ref="K17" si="3">SUM(K7:K9,K11:K16)</f>
-        <v>0</v>
-      </c>
-      <c r="L17" s="16">
-        <f t="shared" ref="L17" si="4">SUM(L7:L9,L11:L16)</f>
-        <v>0</v>
-      </c>
-      <c r="M17" s="16">
-        <f t="shared" ref="M17" si="5">SUM(M7:M9,M11:M16)</f>
-        <v>0</v>
-      </c>
-      <c r="N17" s="16">
-        <f t="shared" ref="N17" si="6">SUM(N7:N9,N11:N16)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" ref="J17" si="5">SUM(J7:J9,J11:J16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="E18" s="2"/>
@@ -1146,14 +1061,10 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1165,56 +1076,43 @@
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M21" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E23" s="12"/>
       <c r="H23" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="I25" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="8">
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:J4"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E2:J2"/>
     <mergeCell ref="E3:J3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
   </mergeCells>
   <pageMargins left="0.2" right="0.2" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>